<commit_message>
Added shell and speedup
</commit_message>
<xml_diff>
--- a/app/webroot/some_excel_file.xlsx
+++ b/app/webroot/some_excel_file.xlsx
@@ -398,16 +398,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.94168277205641</v>
+        <v>0.82738351924175</v>
       </c>
       <c r="C2">
-        <v>0.93996625578492</v>
+        <v>0.8153838604151</v>
       </c>
       <c r="D2">
-        <v>0.94219289291222</v>
+        <v>0.88056996714544</v>
       </c>
       <c r="E2">
-        <v>0.90307608148135</v>
+        <v>0.81892111811686</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -415,16 +415,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.95442940248047</v>
+        <v>0.86770998809498</v>
       </c>
       <c r="C3">
-        <v>0.94776926634972</v>
+        <v>0.81285776754473</v>
       </c>
       <c r="D3">
-        <v>0.96080353686277</v>
+        <v>0.87371640094123</v>
       </c>
       <c r="E3">
-        <v>0.90394243198997</v>
+        <v>0.83344827633768</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -432,16 +432,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.96381608071244</v>
+        <v>0.8845373489403</v>
       </c>
       <c r="C4">
-        <v>0.94801008403532</v>
+        <v>0.82696200048912</v>
       </c>
       <c r="D4">
-        <v>0.95942407749405</v>
+        <v>0.88227355876314</v>
       </c>
       <c r="E4">
-        <v>0.89537531807733</v>
+        <v>0.87254397919085</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -449,16 +449,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.96575790049189</v>
+        <v>0.88899031765418</v>
       </c>
       <c r="C5">
-        <v>0.95568535618658</v>
+        <v>0.81924568196412</v>
       </c>
       <c r="D5">
-        <v>0.96293169520886</v>
+        <v>0.89617491395655</v>
       </c>
       <c r="E5">
-        <v>0.89996608121951</v>
+        <v>0.8704875235578</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -466,16 +466,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.95532086166794</v>
+        <v>0.90897165768578</v>
       </c>
       <c r="C6">
-        <v>0.94827611025011</v>
+        <v>0.83034435195377</v>
       </c>
       <c r="D6">
-        <v>0.96480229611024</v>
+        <v>0.88149220963809</v>
       </c>
       <c r="E6">
-        <v>0.90598120220819</v>
+        <v>0.84750232386965</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -483,16 +483,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.96075246291528</v>
+        <v>0.89324036302584</v>
       </c>
       <c r="C7">
-        <v>0.95588465592673</v>
+        <v>0.84024424199975</v>
       </c>
       <c r="D7">
-        <v>0.96356731320594</v>
+        <v>0.87828913846631</v>
       </c>
       <c r="E7">
-        <v>0.88755269474818</v>
+        <v>0.87154701734997</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -500,16 +500,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.96561882519567</v>
+        <v>0.88000390920867</v>
       </c>
       <c r="C8">
-        <v>0.96239173187119</v>
+        <v>0.81118570577442</v>
       </c>
       <c r="D8">
-        <v>0.96997611808574</v>
+        <v>0.88199862548456</v>
       </c>
       <c r="E8">
-        <v>0.9058451320376</v>
+        <v>0.87900332263319</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -517,16 +517,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.96018396328718</v>
+        <v>0.89382350518692</v>
       </c>
       <c r="C9">
-        <v>0.95960532342025</v>
+        <v>0.84053279048134</v>
       </c>
       <c r="D9">
-        <v>0.96778116739991</v>
+        <v>0.88990550290693</v>
       </c>
       <c r="E9">
-        <v>0.9036300224266</v>
+        <v>0.87739007628422</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -534,16 +534,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.96474442790152</v>
+        <v>0.88387486895669</v>
       </c>
       <c r="C10">
-        <v>0.96005827926694</v>
+        <v>0.86260845777312</v>
       </c>
       <c r="D10">
-        <v>0.96461660455562</v>
+        <v>0.8898713420691</v>
       </c>
       <c r="E10">
-        <v>0.89713360428238</v>
+        <v>0.88376230656661</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -551,16 +551,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.96565935667353</v>
+        <v>0.86780374744058</v>
       </c>
       <c r="C11">
-        <v>0.95096412489008</v>
+        <v>0.82790669460194</v>
       </c>
       <c r="D11">
-        <v>0.96525207529975</v>
+        <v>0.87609751653224</v>
       </c>
       <c r="E11">
-        <v>0.90578647105516</v>
+        <v>0.86563577545383</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -568,16 +568,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.95828307536065</v>
+        <v>0.87366018903715</v>
       </c>
       <c r="C12">
-        <v>0.95284933766868</v>
+        <v>0.82473360730645</v>
       </c>
       <c r="D12">
-        <v>0.95896265787779</v>
+        <v>0.88008032699229</v>
       </c>
       <c r="E12">
-        <v>0.89560783214498</v>
+        <v>0.8690502179098</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -585,16 +585,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.95675290622976</v>
+        <v>0.88598252369098</v>
       </c>
       <c r="C13">
-        <v>0.95324719889051</v>
+        <v>0.85441828256267</v>
       </c>
       <c r="D13">
-        <v>0.9606002030208</v>
+        <v>0.89124005269834</v>
       </c>
       <c r="E13">
-        <v>0.89310941234006</v>
+        <v>0.8415965991997</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -602,16 +602,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.96277423757815</v>
+        <v>0.87019362970145</v>
       </c>
       <c r="C14">
-        <v>0.95367415971005</v>
+        <v>0.79936937037447</v>
       </c>
       <c r="D14">
-        <v>0.96339054522791</v>
+        <v>0.87604356286468</v>
       </c>
       <c r="E14">
-        <v>0.90735847059045</v>
+        <v>0.85647534002307</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -619,16 +619,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.9595446479379</v>
+        <v>0.8852567096839</v>
       </c>
       <c r="C15">
-        <v>0.95148440812167</v>
+        <v>0.83050164791447</v>
       </c>
       <c r="D15">
-        <v>0.96476875178397</v>
+        <v>0.87868279899939</v>
       </c>
       <c r="E15">
-        <v>0.90304953369251</v>
+        <v>0.84676228046345</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -636,16 +636,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.96296771824635</v>
+        <v>0.87557482896458</v>
       </c>
       <c r="C16">
-        <v>0.95370879418885</v>
+        <v>0.8144029109035</v>
       </c>
       <c r="D16">
-        <v>0.96544701092054</v>
+        <v>0.8779112034923</v>
       </c>
       <c r="E16">
-        <v>0.89755746619291</v>
+        <v>0.86232957467933</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -653,16 +653,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.9546032789981</v>
+        <v>0.88400720488157</v>
       </c>
       <c r="C17">
-        <v>0.94589832795142</v>
+        <v>0.81139387453276</v>
       </c>
       <c r="D17">
-        <v>0.95604436480163</v>
+        <v>0.87377949960447</v>
       </c>
       <c r="E17">
-        <v>0.90367464497116</v>
+        <v>0.84064962183312</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -670,16 +670,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.9533360702713</v>
+        <v>0.86902869913562</v>
       </c>
       <c r="C18">
-        <v>0.94696681328839</v>
+        <v>0.80519938234008</v>
       </c>
       <c r="D18">
-        <v>0.96193262508825</v>
+        <v>0.87831569256412</v>
       </c>
       <c r="E18">
-        <v>0.90442474398668</v>
+        <v>0.84081746470917</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -687,16 +687,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.96074708294631</v>
+        <v>0.87107091843847</v>
       </c>
       <c r="C19">
-        <v>0.94515287063825</v>
+        <v>0.83802110030358</v>
       </c>
       <c r="D19">
-        <v>0.96568665639217</v>
+        <v>0.87164616302665</v>
       </c>
       <c r="E19">
-        <v>0.89314103179923</v>
+        <v>0.85393653214292</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -704,16 +704,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.95436113884269</v>
+        <v>0.87766205322</v>
       </c>
       <c r="C20">
-        <v>0.94950444933844</v>
+        <v>0.82018698986832</v>
       </c>
       <c r="D20">
-        <v>0.96123671110926</v>
+        <v>0.86773765006325</v>
       </c>
       <c r="E20">
-        <v>0.90429354052656</v>
+        <v>0.83815661593337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>